<commit_message>
Added new TC TC_Name_2
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Master_Sheet.xlsx
+++ b/src/test/resources/testData/Master_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BYMAT_Automation\WorkSpace\WorkSpace_Photon\SeleniumTraining_B13_MVN\src\test\resources\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06295B7-EE55-459F-91C1-9EB7EDB08528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D940CAF7-FA9B-4C9B-8493-A4B0980ED15E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="20" windowWidth="19180" windowHeight="10060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test_Cases" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="45">
   <si>
     <t xml:space="preserve">Sr. No </t>
   </si>
@@ -73,9 +73,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>Test_Case_04</t>
-  </si>
-  <si>
     <t>Test_Case_05</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>VerifyHomePageOfBymatAutomation1</t>
+  </si>
+  <si>
+    <t>RegisterUserForTheSeleniumTraining2</t>
   </si>
 </sst>
 </file>
@@ -540,7 +540,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -562,7 +562,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
@@ -570,13 +570,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -584,13 +584,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -598,13 +598,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -612,19 +612,21 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>4</v>
@@ -636,7 +638,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>4</v>
@@ -648,7 +650,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>4</v>
@@ -660,7 +662,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>4</v>
@@ -672,7 +674,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>4</v>
@@ -684,7 +686,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>4</v>
@@ -696,7 +698,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>4</v>
@@ -717,10 +719,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4668CBAB-C452-40CE-A283-6DB616929218}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -735,7 +737,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -749,10 +751,10 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>8</v>
@@ -766,16 +768,16 @@
         <v>13</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>11</v>
@@ -786,7 +788,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -800,10 +802,10 @@
         <v>7</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>8</v>
@@ -817,16 +819,16 @@
         <v>13</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>11</v>
@@ -837,19 +839,19 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>11</v>
@@ -860,19 +862,19 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>11</v>
@@ -883,7 +885,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
@@ -897,10 +899,10 @@
         <v>7</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>8</v>
@@ -914,16 +916,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>11</v>
@@ -934,7 +936,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
@@ -948,10 +950,10 @@
         <v>7</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>8</v>
@@ -965,21 +967,72 @@
         <v>13</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F17" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G17" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="3" t="s">
         <v>12</v>
       </c>
     </row>
@@ -991,8 +1044,9 @@
     <hyperlink ref="C9" r:id="rId4" xr:uid="{36DD5D89-36CA-4B9A-A9D1-6373DE784C51}"/>
     <hyperlink ref="C13" r:id="rId5" xr:uid="{3813EA18-F801-44A7-AC06-20BB828F6F03}"/>
     <hyperlink ref="C17" r:id="rId6" xr:uid="{D751F7E4-9179-46D7-82B5-6739CD8927D5}"/>
+    <hyperlink ref="C21" r:id="rId7" xr:uid="{64DD788C-E260-4959-BE67-B2E162F08957}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
</xml_diff>